<commit_message>
Rezolvat bug oprire de siguranta
</commit_message>
<xml_diff>
--- a/Calibrare DHT11.xlsx
+++ b/Calibrare DHT11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IOTProject_Firebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF39544C-2E0A-4144-890A-FF5F7F8D1A40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D459A50-E782-49ED-8578-0DC8CE3B5C31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{90D7E0D1-89C5-48C5-97C3-ED0B9593B70E}"/>
   </bookViews>
@@ -270,7 +270,7 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -282,10 +282,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -644,7 +644,7 @@
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -656,10 +656,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1018,7 +1018,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1033,7 +1033,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1392,7 +1392,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.1</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1407,7 +1407,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4271,8 +4271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0E9EB9-1764-43B7-B96C-480FDC483630}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4297,7 +4297,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F2" s="3">
         <v>20</v>
@@ -4310,16 +4310,16 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I3">
         <v>20</v>
@@ -4360,7 +4360,7 @@
         <v>63</v>
       </c>
       <c r="C12" s="2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F12">
         <v>21</v>
@@ -4372,16 +4372,16 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F13">
-        <v>21.1</v>
+        <v>24</v>
       </c>
       <c r="G13">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I13">
         <v>21</v>

</xml_diff>